<commit_message>
Added percentage of youth and senior registered voters
</commit_message>
<xml_diff>
--- a/incomeED.xlsx
+++ b/incomeED.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alber\Downloads\Stat382\Project4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71A8266-98DE-472C-BC03-7DBBD9F4E714}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBBC8B4A-C6ED-4651-B4A6-C23A37F31999}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{FB97F738-EA3E-4A2B-82FF-4402BAE6696D}"/>
   </bookViews>
@@ -883,16 +883,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05BF4AFF-B23E-4E53-A5FE-D0F4203342A7}">
-  <dimension ref="A1:G162"/>
+  <dimension ref="A1:G160"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+      <selection activeCell="A3" activeCellId="1" sqref="A2:XFD2 A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="7" max="7" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="15.7109375" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" customWidth="1"/>
+    <col min="6" max="6" width="17" customWidth="1"/>
+    <col min="7" max="7" width="17.5703125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -918,1841 +922,1887 @@
         <v>161</v>
       </c>
     </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2">
+        <v>18977</v>
+      </c>
+      <c r="C2">
+        <v>36155</v>
+      </c>
+      <c r="D2">
+        <v>46005</v>
+      </c>
+      <c r="E2">
+        <v>18236</v>
+      </c>
+      <c r="F2">
+        <v>6969</v>
+      </c>
+      <c r="G2">
+        <v>17.600000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3">
+        <v>15456</v>
+      </c>
+      <c r="C3">
+        <v>33834</v>
+      </c>
+      <c r="D3">
+        <v>34859</v>
+      </c>
+      <c r="E3">
+        <v>8375</v>
+      </c>
+      <c r="F3">
+        <v>2983</v>
+      </c>
+      <c r="G3">
+        <v>13.8</v>
+      </c>
+    </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B4">
-        <v>18977</v>
+        <v>17110</v>
       </c>
       <c r="C4">
-        <v>36155</v>
+        <v>31429</v>
       </c>
       <c r="D4">
-        <v>46005</v>
+        <v>45442</v>
       </c>
       <c r="E4">
-        <v>18236</v>
+        <v>11096</v>
       </c>
       <c r="F4">
-        <v>6969</v>
+        <v>4214</v>
       </c>
       <c r="G4">
-        <v>17.600000000000001</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B5">
-        <v>15456</v>
+        <v>16379</v>
       </c>
       <c r="C5">
-        <v>33834</v>
+        <v>27462</v>
       </c>
       <c r="D5">
-        <v>34859</v>
+        <v>42585</v>
       </c>
       <c r="E5">
-        <v>8375</v>
+        <v>3451</v>
       </c>
       <c r="F5">
-        <v>2983</v>
+        <v>1372</v>
       </c>
       <c r="G5">
-        <v>13.8</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="B6">
-        <v>17110</v>
+        <v>17488</v>
       </c>
       <c r="C6">
-        <v>31429</v>
+        <v>37237</v>
       </c>
       <c r="D6">
-        <v>45442</v>
+        <v>47714</v>
       </c>
       <c r="E6">
-        <v>11096</v>
+        <v>45720</v>
       </c>
       <c r="F6">
-        <v>4214</v>
+        <v>16788</v>
       </c>
       <c r="G6">
-        <v>21.3</v>
+        <v>25.5</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B7">
-        <v>16379</v>
+        <v>19497</v>
       </c>
       <c r="C7">
-        <v>27462</v>
+        <v>40455</v>
       </c>
       <c r="D7">
-        <v>42585</v>
+        <v>48606</v>
       </c>
       <c r="E7">
-        <v>3451</v>
+        <v>18395</v>
       </c>
       <c r="F7">
-        <v>1372</v>
+        <v>6700</v>
       </c>
       <c r="G7">
-        <v>18.8</v>
+        <v>16.899999999999999</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B8">
-        <v>17488</v>
+        <v>20882</v>
       </c>
       <c r="C8">
-        <v>37237</v>
+        <v>48958</v>
       </c>
       <c r="D8">
-        <v>47714</v>
+        <v>55415</v>
       </c>
       <c r="E8">
-        <v>45720</v>
+        <v>69367</v>
       </c>
       <c r="F8">
-        <v>16788</v>
+        <v>23971</v>
       </c>
       <c r="G8">
-        <v>25.5</v>
+        <v>25.6</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B9">
-        <v>19497</v>
+        <v>22241</v>
       </c>
       <c r="C9">
-        <v>40455</v>
+        <v>49216</v>
       </c>
       <c r="D9">
-        <v>48606</v>
+        <v>56281</v>
       </c>
       <c r="E9">
-        <v>18395</v>
+        <v>100157</v>
       </c>
       <c r="F9">
-        <v>6700</v>
+        <v>35782</v>
       </c>
       <c r="G9">
-        <v>16.899999999999999</v>
+        <v>25.6</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B10">
-        <v>20882</v>
+        <v>15529</v>
       </c>
       <c r="C10">
-        <v>48958</v>
+        <v>30134</v>
       </c>
       <c r="D10">
-        <v>55415</v>
+        <v>35868</v>
       </c>
       <c r="E10">
-        <v>69367</v>
+        <v>17634</v>
       </c>
       <c r="F10">
-        <v>23971</v>
+        <v>6794</v>
       </c>
       <c r="G10">
-        <v>25.6</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B11">
-        <v>22241</v>
+        <v>16049</v>
       </c>
       <c r="C11">
-        <v>49216</v>
+        <v>32202</v>
       </c>
       <c r="D11">
-        <v>56281</v>
+        <v>40869</v>
       </c>
       <c r="E11">
-        <v>100157</v>
+        <v>19286</v>
       </c>
       <c r="F11">
-        <v>35782</v>
+        <v>7443</v>
       </c>
       <c r="G11">
-        <v>25.6</v>
+        <v>23</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B12">
-        <v>15529</v>
+        <v>21436</v>
       </c>
       <c r="C12">
-        <v>30134</v>
+        <v>38798</v>
       </c>
       <c r="D12">
-        <v>35868</v>
+        <v>52158</v>
       </c>
       <c r="E12">
-        <v>17634</v>
+        <v>155547</v>
       </c>
       <c r="F12">
-        <v>6794</v>
+        <v>60295</v>
       </c>
       <c r="G12">
-        <v>19.100000000000001</v>
+        <v>31</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B13">
-        <v>16049</v>
+        <v>18960</v>
       </c>
       <c r="C13">
-        <v>32202</v>
+        <v>35661</v>
       </c>
       <c r="D13">
-        <v>40869</v>
+        <v>48750</v>
       </c>
       <c r="E13">
-        <v>19286</v>
+        <v>13063</v>
       </c>
       <c r="F13">
-        <v>7443</v>
+        <v>4660</v>
       </c>
       <c r="G13">
-        <v>23</v>
+        <v>24.3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B14">
-        <v>21436</v>
+        <v>18905</v>
       </c>
       <c r="C14">
-        <v>38798</v>
+        <v>37343</v>
       </c>
       <c r="D14">
-        <v>52158</v>
+        <v>43028</v>
       </c>
       <c r="E14">
-        <v>155547</v>
+        <v>18411</v>
       </c>
       <c r="F14">
-        <v>60295</v>
+        <v>6885</v>
       </c>
       <c r="G14">
-        <v>31</v>
+        <v>16.5</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15">
-        <v>18960</v>
+        <v>20346</v>
       </c>
       <c r="C15">
-        <v>35661</v>
+        <v>41309</v>
       </c>
       <c r="D15">
-        <v>48750</v>
+        <v>47599</v>
       </c>
       <c r="E15">
-        <v>13063</v>
+        <v>16243</v>
       </c>
       <c r="F15">
-        <v>4660</v>
+        <v>6457</v>
       </c>
       <c r="G15">
-        <v>24.3</v>
+        <v>19.600000000000001</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B16">
-        <v>18905</v>
+        <v>28365</v>
       </c>
       <c r="C16">
-        <v>37343</v>
+        <v>63244</v>
       </c>
       <c r="D16">
-        <v>43028</v>
+        <v>72118</v>
       </c>
       <c r="E16">
-        <v>18411</v>
+        <v>30233</v>
       </c>
       <c r="F16">
-        <v>6885</v>
+        <v>10738</v>
       </c>
       <c r="G16">
-        <v>16.5</v>
+        <v>42.3</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B17">
-        <v>20346</v>
+        <v>17812</v>
       </c>
       <c r="C17">
-        <v>41309</v>
+        <v>34327</v>
       </c>
       <c r="D17">
-        <v>47599</v>
+        <v>51904</v>
       </c>
       <c r="E17">
-        <v>16243</v>
+        <v>70217</v>
       </c>
       <c r="F17">
-        <v>6457</v>
+        <v>25575</v>
       </c>
       <c r="G17">
-        <v>19.600000000000001</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B18">
-        <v>28365</v>
+        <v>15934</v>
       </c>
       <c r="C18">
-        <v>63244</v>
+        <v>33155</v>
       </c>
       <c r="D18">
-        <v>72118</v>
+        <v>41659</v>
       </c>
       <c r="E18">
-        <v>30233</v>
+        <v>23316</v>
       </c>
       <c r="F18">
-        <v>10738</v>
+        <v>8533</v>
       </c>
       <c r="G18">
-        <v>42.3</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B19">
-        <v>17812</v>
+        <v>20963</v>
       </c>
       <c r="C19">
-        <v>34327</v>
+        <v>52257</v>
       </c>
       <c r="D19">
-        <v>51904</v>
+        <v>59511</v>
       </c>
       <c r="E19">
-        <v>70217</v>
+        <v>23655</v>
       </c>
       <c r="F19">
-        <v>25575</v>
+        <v>7881</v>
       </c>
       <c r="G19">
-        <v>35.9</v>
+        <v>14.1</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B20">
-        <v>15934</v>
+        <v>12452</v>
       </c>
       <c r="C20">
-        <v>33155</v>
+        <v>30522</v>
       </c>
       <c r="D20">
-        <v>41659</v>
+        <v>37309</v>
       </c>
       <c r="E20">
-        <v>23316</v>
+        <v>6694</v>
       </c>
       <c r="F20">
-        <v>8533</v>
+        <v>2002</v>
       </c>
       <c r="G20">
-        <v>19.100000000000001</v>
+        <v>14.4</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B21">
-        <v>20963</v>
+        <v>22022</v>
       </c>
       <c r="C21">
-        <v>52257</v>
+        <v>49230</v>
       </c>
       <c r="D21">
-        <v>59511</v>
+        <v>57366</v>
       </c>
       <c r="E21">
-        <v>23655</v>
+        <v>50513</v>
       </c>
       <c r="F21">
-        <v>7881</v>
+        <v>18047</v>
       </c>
       <c r="G21">
-        <v>14.1</v>
+        <v>32.6</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B22">
-        <v>12452</v>
+        <v>16068</v>
       </c>
       <c r="C22">
-        <v>30522</v>
+        <v>35828</v>
       </c>
       <c r="D22">
-        <v>37309</v>
+        <v>39105</v>
       </c>
       <c r="E22">
-        <v>6694</v>
+        <v>10998</v>
       </c>
       <c r="F22">
-        <v>2002</v>
+        <v>4041</v>
       </c>
       <c r="G22">
-        <v>14.4</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B23">
-        <v>22022</v>
+        <v>20523</v>
       </c>
       <c r="C23">
-        <v>49230</v>
+        <v>45559</v>
       </c>
       <c r="D23">
-        <v>57366</v>
+        <v>53703</v>
       </c>
       <c r="E23">
-        <v>50513</v>
+        <v>110527</v>
       </c>
       <c r="F23">
-        <v>18047</v>
+        <v>39187</v>
       </c>
       <c r="G23">
-        <v>32.6</v>
+        <v>23.7</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B24">
-        <v>16068</v>
+        <v>22563</v>
       </c>
       <c r="C24">
-        <v>35828</v>
+        <v>46544</v>
       </c>
       <c r="D24">
-        <v>39105</v>
+        <v>54796</v>
       </c>
       <c r="E24">
-        <v>10998</v>
+        <v>63942</v>
       </c>
       <c r="F24">
-        <v>4041</v>
+        <v>24475</v>
       </c>
       <c r="G24">
-        <v>21.6</v>
+        <v>29.8</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B25">
-        <v>20523</v>
+        <v>16652</v>
       </c>
       <c r="C25">
-        <v>45559</v>
+        <v>40850</v>
       </c>
       <c r="D25">
-        <v>53703</v>
+        <v>45913</v>
       </c>
       <c r="E25">
-        <v>110527</v>
+        <v>12171</v>
       </c>
       <c r="F25">
-        <v>39187</v>
+        <v>3927</v>
       </c>
       <c r="G25">
-        <v>23.7</v>
+        <v>15.7</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B26">
-        <v>22563</v>
+        <v>25397</v>
       </c>
       <c r="C26">
-        <v>46544</v>
+        <v>44928</v>
       </c>
       <c r="D26">
-        <v>54796</v>
+        <v>54933</v>
       </c>
       <c r="E26">
-        <v>63942</v>
+        <v>265128</v>
       </c>
       <c r="F26">
-        <v>24475</v>
+        <v>103038</v>
       </c>
       <c r="G26">
-        <v>29.8</v>
+        <v>39.700000000000003</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B27">
-        <v>16652</v>
+        <v>22202</v>
       </c>
       <c r="C27">
-        <v>40850</v>
+        <v>51089</v>
       </c>
       <c r="D27">
-        <v>45913</v>
+        <v>55745</v>
       </c>
       <c r="E27">
-        <v>12171</v>
+        <v>11267</v>
       </c>
       <c r="F27">
-        <v>3927</v>
+        <v>2686</v>
       </c>
       <c r="G27">
-        <v>15.7</v>
+        <v>37.799999999999997</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28">
-        <v>25397</v>
+        <v>15158</v>
       </c>
       <c r="C28">
-        <v>44928</v>
+        <v>32419</v>
       </c>
       <c r="D28">
-        <v>54933</v>
+        <v>39037</v>
       </c>
       <c r="E28">
-        <v>265128</v>
+        <v>26015</v>
       </c>
       <c r="F28">
-        <v>103038</v>
+        <v>9548</v>
       </c>
       <c r="G28">
-        <v>39.700000000000003</v>
+        <v>16</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B29">
-        <v>22202</v>
+        <v>30217</v>
       </c>
       <c r="C29">
-        <v>51089</v>
+        <v>66320</v>
       </c>
       <c r="D29">
-        <v>55745</v>
+        <v>77190</v>
       </c>
       <c r="E29">
-        <v>11267</v>
+        <v>214346</v>
       </c>
       <c r="F29">
-        <v>2686</v>
+        <v>75936</v>
       </c>
       <c r="G29">
-        <v>37.799999999999997</v>
+        <v>42.5</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="B30">
-        <v>15158</v>
+        <v>19839</v>
       </c>
       <c r="C30">
-        <v>32419</v>
+        <v>34253</v>
       </c>
       <c r="D30">
-        <v>39037</v>
+        <v>51687</v>
       </c>
       <c r="E30">
-        <v>26015</v>
+        <v>116714</v>
       </c>
       <c r="F30">
-        <v>9548</v>
+        <v>45414</v>
       </c>
       <c r="G30">
-        <v>16</v>
+        <v>47</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="B31">
-        <v>30217</v>
+        <v>13353</v>
       </c>
       <c r="C31">
-        <v>66320</v>
+        <v>26250</v>
       </c>
       <c r="D31">
-        <v>77190</v>
+        <v>31354</v>
       </c>
       <c r="E31">
-        <v>214346</v>
+        <v>3183</v>
       </c>
       <c r="F31">
-        <v>75936</v>
+        <v>1331</v>
       </c>
       <c r="G31">
-        <v>42.5</v>
+        <v>14.6</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B32">
-        <v>19839</v>
+        <v>18958</v>
       </c>
       <c r="C32">
-        <v>34253</v>
+        <v>43311</v>
       </c>
       <c r="D32">
-        <v>51687</v>
+        <v>48064</v>
       </c>
       <c r="E32">
-        <v>116714</v>
+        <v>259424</v>
       </c>
       <c r="F32">
-        <v>45414</v>
+        <v>90633</v>
       </c>
       <c r="G32">
-        <v>47</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="B33">
-        <v>13353</v>
+        <v>16709</v>
       </c>
       <c r="C33">
-        <v>26250</v>
+        <v>31963</v>
       </c>
       <c r="D33">
-        <v>31354</v>
+        <v>45350</v>
       </c>
       <c r="E33">
-        <v>3183</v>
+        <v>6798</v>
       </c>
       <c r="F33">
-        <v>1331</v>
+        <v>2572</v>
       </c>
       <c r="G33">
-        <v>14.6</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="B34">
-        <v>18958</v>
+        <v>33110</v>
       </c>
       <c r="C34">
-        <v>43311</v>
+        <v>65522</v>
       </c>
       <c r="D34">
-        <v>48064</v>
+        <v>78920</v>
       </c>
       <c r="E34">
-        <v>259424</v>
+        <v>688078</v>
       </c>
       <c r="F34">
-        <v>90633</v>
+        <v>260056</v>
       </c>
       <c r="G34">
-        <v>26.9</v>
+        <v>52.2</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B35">
-        <v>16709</v>
+        <v>16664</v>
       </c>
       <c r="C35">
-        <v>31963</v>
+        <v>35202</v>
       </c>
       <c r="D35">
-        <v>45350</v>
+        <v>39880</v>
       </c>
       <c r="E35">
-        <v>6798</v>
+        <v>42356</v>
       </c>
       <c r="F35">
-        <v>2572</v>
+        <v>14817</v>
       </c>
       <c r="G35">
-        <v>19.899999999999999</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B36">
-        <v>33110</v>
+        <v>17362</v>
       </c>
       <c r="C36">
-        <v>65522</v>
+        <v>32902</v>
       </c>
       <c r="D36">
-        <v>78920</v>
+        <v>39086</v>
       </c>
       <c r="E36">
-        <v>688078</v>
+        <v>45498</v>
       </c>
       <c r="F36">
-        <v>260056</v>
+        <v>16317</v>
       </c>
       <c r="G36">
-        <v>52.2</v>
+        <v>19.100000000000001</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="B37">
-        <v>16664</v>
+        <v>29479</v>
       </c>
       <c r="C37">
-        <v>35202</v>
+        <v>66333</v>
       </c>
       <c r="D37">
-        <v>39880</v>
+        <v>74426</v>
       </c>
       <c r="E37">
-        <v>42356</v>
+        <v>124053</v>
       </c>
       <c r="F37">
-        <v>14817</v>
+        <v>44898</v>
       </c>
       <c r="G37">
-        <v>21.3</v>
+        <v>45.6</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="B38">
-        <v>17362</v>
+        <v>16528</v>
       </c>
       <c r="C38">
-        <v>32902</v>
+        <v>31390</v>
       </c>
       <c r="D38">
-        <v>39086</v>
+        <v>37352</v>
       </c>
       <c r="E38">
-        <v>45498</v>
+        <v>17212</v>
       </c>
       <c r="F38">
-        <v>16317</v>
+        <v>6339</v>
       </c>
       <c r="G38">
-        <v>19.100000000000001</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B39">
-        <v>29479</v>
+        <v>26161</v>
       </c>
       <c r="C39">
-        <v>66333</v>
+        <v>61550</v>
       </c>
       <c r="D39">
-        <v>74426</v>
+        <v>68469</v>
       </c>
       <c r="E39">
-        <v>124053</v>
+        <v>127317</v>
       </c>
       <c r="F39">
-        <v>44898</v>
+        <v>45673</v>
       </c>
       <c r="G39">
-        <v>45.6</v>
+        <v>35.1</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B40">
-        <v>16528</v>
+        <v>20692</v>
       </c>
       <c r="C40">
-        <v>31390</v>
+        <v>37062</v>
       </c>
       <c r="D40">
-        <v>37352</v>
+        <v>48623</v>
       </c>
       <c r="E40">
-        <v>17212</v>
+        <v>12630</v>
       </c>
       <c r="F40">
-        <v>6339</v>
+        <v>4822</v>
       </c>
       <c r="G40">
-        <v>20.8</v>
+        <v>19.3</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B41">
-        <v>26161</v>
+        <v>17187</v>
       </c>
       <c r="C41">
-        <v>61550</v>
+        <v>29960</v>
       </c>
       <c r="D41">
-        <v>68469</v>
+        <v>41616</v>
       </c>
       <c r="E41">
-        <v>127317</v>
+        <v>23439</v>
       </c>
       <c r="F41">
-        <v>45673</v>
+        <v>9079</v>
       </c>
       <c r="G41">
-        <v>35.1</v>
+        <v>20.399999999999999</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="B42">
-        <v>20692</v>
+        <v>20168</v>
       </c>
       <c r="C42">
-        <v>37062</v>
+        <v>39760</v>
       </c>
       <c r="D42">
-        <v>48623</v>
+        <v>48881</v>
       </c>
       <c r="E42">
-        <v>12630</v>
+        <v>16633</v>
       </c>
       <c r="F42">
-        <v>4822</v>
+        <v>6291</v>
       </c>
       <c r="G42">
-        <v>19.3</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B43">
-        <v>17187</v>
+        <v>25557</v>
       </c>
       <c r="C43">
-        <v>29960</v>
+        <v>51128</v>
       </c>
       <c r="D43">
-        <v>41616</v>
+        <v>60236</v>
       </c>
       <c r="E43">
-        <v>23439</v>
+        <v>22330</v>
       </c>
       <c r="F43">
-        <v>9079</v>
+        <v>8433</v>
       </c>
       <c r="G43">
-        <v>20.399999999999999</v>
+        <v>35.5</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="B44">
-        <v>20168</v>
+        <v>17833</v>
       </c>
       <c r="C44">
-        <v>39760</v>
+        <v>33297</v>
       </c>
       <c r="D44">
-        <v>48881</v>
+        <v>44322</v>
       </c>
       <c r="E44">
-        <v>16633</v>
+        <v>27842</v>
       </c>
       <c r="F44">
-        <v>6291</v>
+        <v>10390</v>
       </c>
       <c r="G44">
-        <v>23.1</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="B45">
-        <v>25557</v>
+        <v>28412</v>
       </c>
       <c r="C45">
-        <v>51128</v>
+        <v>51349</v>
       </c>
       <c r="D45">
-        <v>60236</v>
+        <v>60718</v>
       </c>
       <c r="E45">
-        <v>22330</v>
+        <v>691893</v>
       </c>
       <c r="F45">
-        <v>8433</v>
+        <v>271809</v>
       </c>
       <c r="G45">
-        <v>35.5</v>
+        <v>48.4</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B46">
-        <v>17833</v>
+        <v>16288</v>
       </c>
       <c r="C46">
-        <v>33297</v>
+        <v>33580</v>
       </c>
       <c r="D46">
-        <v>44322</v>
+        <v>46460</v>
       </c>
       <c r="E46">
-        <v>27842</v>
+        <v>21796</v>
       </c>
       <c r="F46">
-        <v>10390</v>
+        <v>8177</v>
       </c>
       <c r="G46">
-        <v>23.3</v>
+        <v>21.6</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="B47">
-        <v>28412</v>
+        <v>14871</v>
       </c>
       <c r="C47">
-        <v>51349</v>
+        <v>31038</v>
       </c>
       <c r="D47">
-        <v>60718</v>
+        <v>39622</v>
       </c>
       <c r="E47">
-        <v>691893</v>
+        <v>14918</v>
       </c>
       <c r="F47">
-        <v>271809</v>
+        <v>5286</v>
       </c>
       <c r="G47">
-        <v>48.4</v>
+        <v>16.399999999999999</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="B48">
-        <v>16288</v>
+        <v>19210</v>
       </c>
       <c r="C48">
-        <v>33580</v>
+        <v>32435</v>
       </c>
       <c r="D48">
-        <v>46460</v>
+        <v>39951</v>
       </c>
       <c r="E48">
-        <v>21796</v>
+        <v>94565</v>
       </c>
       <c r="F48">
-        <v>8177</v>
+        <v>36508</v>
       </c>
       <c r="G48">
-        <v>21.6</v>
+        <v>27.3</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B49">
-        <v>14871</v>
+        <v>24515</v>
       </c>
       <c r="C49">
-        <v>31038</v>
+        <v>55852</v>
       </c>
       <c r="D49">
-        <v>39622</v>
+        <v>62977</v>
       </c>
       <c r="E49">
-        <v>14918</v>
+        <v>132403</v>
       </c>
       <c r="F49">
-        <v>5286</v>
+        <v>46624</v>
       </c>
       <c r="G49">
-        <v>16.399999999999999</v>
+        <v>33.700000000000003</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B50">
-        <v>19210</v>
+        <v>16330</v>
       </c>
       <c r="C50">
-        <v>32435</v>
+        <v>26928</v>
       </c>
       <c r="D50">
-        <v>39951</v>
+        <v>40238</v>
       </c>
       <c r="E50">
-        <v>94565</v>
+        <v>11008</v>
       </c>
       <c r="F50">
-        <v>36508</v>
+        <v>4228</v>
       </c>
       <c r="G50">
-        <v>27.3</v>
+        <v>21.7</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="B51">
-        <v>24515</v>
+        <v>14201</v>
       </c>
       <c r="C51">
-        <v>55852</v>
+        <v>32390</v>
       </c>
       <c r="D51">
-        <v>62977</v>
+        <v>33664</v>
       </c>
       <c r="E51">
-        <v>132403</v>
+        <v>4034</v>
       </c>
       <c r="F51">
-        <v>46624</v>
+        <v>1329</v>
       </c>
       <c r="G51">
-        <v>33.700000000000003</v>
+        <v>14</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B52">
-        <v>16330</v>
+        <v>23465</v>
       </c>
       <c r="C52">
-        <v>26928</v>
+        <v>56903</v>
       </c>
       <c r="D52">
-        <v>40238</v>
+        <v>63277</v>
       </c>
       <c r="E52">
-        <v>11008</v>
+        <v>52250</v>
       </c>
       <c r="F52">
-        <v>4228</v>
+        <v>18092</v>
       </c>
       <c r="G52">
-        <v>21.7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="B53">
-        <v>14201</v>
+        <v>17100</v>
       </c>
       <c r="C53">
-        <v>32390</v>
+        <v>30543</v>
       </c>
       <c r="D53">
-        <v>33664</v>
+        <v>35550</v>
       </c>
       <c r="E53">
-        <v>4034</v>
+        <v>20166</v>
       </c>
       <c r="F53">
-        <v>1329</v>
+        <v>8063</v>
       </c>
       <c r="G53">
-        <v>14</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B54">
-        <v>23465</v>
+        <v>16076</v>
       </c>
       <c r="C54">
-        <v>56903</v>
+        <v>30205</v>
       </c>
       <c r="D54">
-        <v>63277</v>
+        <v>36402</v>
       </c>
       <c r="E54">
-        <v>52250</v>
+        <v>22598</v>
       </c>
       <c r="F54">
-        <v>18092</v>
+        <v>8430</v>
       </c>
       <c r="G54">
-        <v>26</v>
+        <v>17.8</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B55">
-        <v>17100</v>
+        <v>19072</v>
       </c>
       <c r="C55">
-        <v>30543</v>
+        <v>40796</v>
       </c>
       <c r="D55">
-        <v>35550</v>
+        <v>45938</v>
       </c>
       <c r="E55">
-        <v>20166</v>
+        <v>11000</v>
       </c>
       <c r="F55">
-        <v>8063</v>
+        <v>4033</v>
       </c>
       <c r="G55">
-        <v>17.399999999999999</v>
+        <v>20.5</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="B56">
-        <v>16076</v>
+        <v>21103</v>
       </c>
       <c r="C56">
-        <v>30205</v>
+        <v>34145</v>
       </c>
       <c r="D56">
-        <v>36402</v>
+        <v>41422</v>
       </c>
       <c r="E56">
-        <v>22598</v>
+        <v>23682</v>
       </c>
       <c r="F56">
-        <v>8430</v>
+        <v>10187</v>
       </c>
       <c r="G56">
-        <v>17.8</v>
+        <v>24.9</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B57">
-        <v>19072</v>
+        <v>35076</v>
       </c>
       <c r="C57">
-        <v>40796</v>
+        <v>82216</v>
       </c>
       <c r="D57">
-        <v>45938</v>
+        <v>92976</v>
       </c>
       <c r="E57">
-        <v>11000</v>
+        <v>106567</v>
       </c>
       <c r="F57">
-        <v>4033</v>
+        <v>38167</v>
       </c>
       <c r="G57">
-        <v>20.5</v>
+        <v>53.4</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B58">
-        <v>21103</v>
+        <v>20640</v>
       </c>
       <c r="C58">
-        <v>34145</v>
+        <v>41066</v>
       </c>
       <c r="D58">
-        <v>41422</v>
+        <v>49310</v>
       </c>
       <c r="E58">
-        <v>23682</v>
+        <v>96317</v>
       </c>
       <c r="F58">
-        <v>10187</v>
+        <v>35930</v>
       </c>
       <c r="G58">
-        <v>24.9</v>
+        <v>26.6</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="B59">
-        <v>35076</v>
+        <v>37211</v>
       </c>
       <c r="C59">
-        <v>82216</v>
+        <v>56709</v>
       </c>
       <c r="D59">
-        <v>92976</v>
+        <v>75579</v>
       </c>
       <c r="E59">
-        <v>106567</v>
+        <v>1010562</v>
       </c>
       <c r="F59">
-        <v>38167</v>
+        <v>376377</v>
       </c>
       <c r="G59">
-        <v>53.4</v>
+        <v>55.3</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B60">
-        <v>20640</v>
+        <v>19276</v>
       </c>
       <c r="C60">
-        <v>41066</v>
+        <v>36739</v>
       </c>
       <c r="D60">
-        <v>49310</v>
+        <v>44667</v>
       </c>
       <c r="E60">
-        <v>96317</v>
+        <v>22084</v>
       </c>
       <c r="F60">
-        <v>35930</v>
+        <v>8540</v>
       </c>
       <c r="G60">
-        <v>26.6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B61">
-        <v>37211</v>
+        <v>35385</v>
       </c>
       <c r="C61">
-        <v>56709</v>
+        <v>87605</v>
       </c>
       <c r="D61">
-        <v>75579</v>
+        <v>96501</v>
       </c>
       <c r="E61">
-        <v>1010562</v>
+        <v>175511</v>
       </c>
       <c r="F61">
-        <v>376377</v>
+        <v>59433</v>
       </c>
       <c r="G61">
-        <v>55.3</v>
+        <v>55.6</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="B62">
-        <v>19276</v>
+        <v>20439</v>
       </c>
       <c r="C62">
-        <v>36739</v>
+        <v>36741</v>
       </c>
       <c r="D62">
-        <v>44667</v>
+        <v>45317</v>
       </c>
       <c r="E62">
-        <v>22084</v>
+        <v>28292</v>
       </c>
       <c r="F62">
-        <v>8540</v>
+        <v>11314</v>
       </c>
       <c r="G62">
-        <v>20</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="B63">
-        <v>35385</v>
+        <v>16844</v>
       </c>
       <c r="C63">
-        <v>87605</v>
+        <v>37149</v>
       </c>
       <c r="D63">
-        <v>96501</v>
+        <v>46283</v>
       </c>
       <c r="E63">
-        <v>175511</v>
+        <v>3082</v>
       </c>
       <c r="F63">
-        <v>59433</v>
+        <v>1162</v>
       </c>
       <c r="G63">
-        <v>55.6</v>
+        <v>12.7</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
       <c r="B64">
-        <v>20439</v>
+        <v>28040</v>
       </c>
       <c r="C64">
-        <v>36741</v>
+        <v>50337</v>
       </c>
       <c r="D64">
-        <v>45317</v>
+        <v>62445</v>
       </c>
       <c r="E64">
-        <v>28292</v>
+        <v>79626</v>
       </c>
       <c r="F64">
-        <v>11314</v>
+        <v>31774</v>
       </c>
       <c r="G64">
-        <v>25.3</v>
+        <v>36.1</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B65">
-        <v>16844</v>
+        <v>18285</v>
       </c>
       <c r="C65">
-        <v>37149</v>
+        <v>40916</v>
       </c>
       <c r="D65">
-        <v>46283</v>
+        <v>47964</v>
       </c>
       <c r="E65">
-        <v>3082</v>
+        <v>55186</v>
       </c>
       <c r="F65">
-        <v>1162</v>
+        <v>19715</v>
       </c>
       <c r="G65">
-        <v>12.7</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B66">
-        <v>28040</v>
+        <v>17785</v>
       </c>
       <c r="C66">
-        <v>50337</v>
+        <v>32247</v>
       </c>
       <c r="D66">
-        <v>62445</v>
+        <v>39159</v>
       </c>
       <c r="E66">
-        <v>79626</v>
+        <v>25011</v>
       </c>
       <c r="F66">
-        <v>31774</v>
+        <v>9418</v>
       </c>
       <c r="G66">
-        <v>36.1</v>
+        <v>21.5</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="B67">
-        <v>18285</v>
+        <v>24943</v>
       </c>
       <c r="C67">
-        <v>40916</v>
+        <v>38513</v>
       </c>
       <c r="D67">
-        <v>47964</v>
+        <v>42307</v>
       </c>
       <c r="E67">
-        <v>55186</v>
+        <v>15994</v>
       </c>
       <c r="F67">
-        <v>19715</v>
+        <v>6519</v>
       </c>
       <c r="G67">
-        <v>18.7</v>
+        <v>30.3</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B68">
-        <v>17785</v>
+        <v>26901</v>
       </c>
       <c r="C68">
-        <v>32247</v>
+        <v>63219</v>
       </c>
       <c r="D68">
-        <v>39159</v>
+        <v>70767</v>
       </c>
       <c r="E68">
-        <v>25011</v>
+        <v>805321</v>
       </c>
       <c r="F68">
-        <v>9418</v>
+        <v>268519</v>
       </c>
       <c r="G68">
-        <v>21.5</v>
+        <v>44</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B69">
-        <v>24943</v>
+        <v>19286</v>
       </c>
       <c r="C69">
-        <v>38513</v>
+        <v>40192</v>
       </c>
       <c r="D69">
-        <v>42307</v>
+        <v>49182</v>
       </c>
       <c r="E69">
-        <v>15994</v>
+        <v>43041</v>
       </c>
       <c r="F69">
-        <v>6519</v>
+        <v>15472</v>
       </c>
       <c r="G69">
-        <v>30.3</v>
+        <v>23.9</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B70">
-        <v>26901</v>
+        <v>23675</v>
       </c>
       <c r="C70">
-        <v>63219</v>
+        <v>50876</v>
       </c>
       <c r="D70">
-        <v>70767</v>
+        <v>57774</v>
       </c>
       <c r="E70">
-        <v>805321</v>
+        <v>179684</v>
       </c>
       <c r="F70">
-        <v>268519</v>
+        <v>60691</v>
       </c>
       <c r="G70">
-        <v>44</v>
+        <v>29.3</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B71">
-        <v>19286</v>
+        <v>10925</v>
       </c>
       <c r="C71">
-        <v>40192</v>
+        <v>22283</v>
       </c>
       <c r="D71">
-        <v>49182</v>
+        <v>27168</v>
       </c>
       <c r="E71">
-        <v>43041</v>
+        <v>9429</v>
       </c>
       <c r="F71">
-        <v>15472</v>
+        <v>3341</v>
       </c>
       <c r="G71">
-        <v>23.9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="B72">
-        <v>23675</v>
+        <v>19033</v>
       </c>
       <c r="C72">
-        <v>50876</v>
+        <v>38996</v>
       </c>
       <c r="D72">
-        <v>57774</v>
+        <v>45339</v>
       </c>
       <c r="E72">
-        <v>179684</v>
+        <v>28780</v>
       </c>
       <c r="F72">
-        <v>60691</v>
+        <v>10757</v>
       </c>
       <c r="G72">
-        <v>29.3</v>
+        <v>19.899999999999999</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B73">
-        <v>10925</v>
+        <v>31073</v>
       </c>
       <c r="C73">
-        <v>22283</v>
+        <v>67018</v>
       </c>
       <c r="D73">
-        <v>27168</v>
+        <v>74457</v>
       </c>
       <c r="E73">
-        <v>9429</v>
+        <v>32024</v>
       </c>
       <c r="F73">
-        <v>3341</v>
+        <v>11823</v>
       </c>
       <c r="G73">
-        <v>15</v>
+        <v>36.299999999999997</v>
       </c>
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B74">
-        <v>19033</v>
+        <v>19124</v>
       </c>
       <c r="C74">
-        <v>38996</v>
+        <v>36109</v>
       </c>
       <c r="D74">
-        <v>45339</v>
+        <v>44451</v>
       </c>
       <c r="E74">
-        <v>28780</v>
+        <v>25213</v>
       </c>
       <c r="F74">
-        <v>10757</v>
+        <v>10121</v>
       </c>
       <c r="G74">
-        <v>19.899999999999999</v>
+        <v>21</v>
       </c>
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="B75">
-        <v>31073</v>
+        <v>18077</v>
       </c>
       <c r="C75">
-        <v>67018</v>
+        <v>42685</v>
       </c>
       <c r="D75">
-        <v>74457</v>
+        <v>47591</v>
       </c>
       <c r="E75">
-        <v>32024</v>
+        <v>11834</v>
       </c>
       <c r="F75">
-        <v>11823</v>
+        <v>4400</v>
       </c>
       <c r="G75">
-        <v>36.299999999999997</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="B76">
-        <v>19124</v>
+        <v>25773</v>
       </c>
       <c r="C76">
-        <v>36109</v>
+        <v>63923</v>
       </c>
       <c r="D76">
-        <v>44451</v>
+        <v>70972</v>
       </c>
       <c r="E76">
-        <v>25213</v>
+        <v>203922</v>
       </c>
       <c r="F76">
-        <v>10121</v>
+        <v>70255</v>
       </c>
       <c r="G76">
-        <v>21</v>
+        <v>26.9</v>
       </c>
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B77">
-        <v>18077</v>
+        <v>25206</v>
       </c>
       <c r="C77">
-        <v>42685</v>
+        <v>55098</v>
       </c>
       <c r="D77">
-        <v>47591</v>
+        <v>67227</v>
       </c>
       <c r="E77">
-        <v>11834</v>
+        <v>139900</v>
       </c>
       <c r="F77">
-        <v>4400</v>
+        <v>53051</v>
       </c>
       <c r="G77">
-        <v>16.3</v>
+        <v>34.4</v>
       </c>
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="B78">
-        <v>25773</v>
+        <v>16561</v>
       </c>
       <c r="C78">
-        <v>63923</v>
+        <v>38376</v>
       </c>
       <c r="D78">
-        <v>70972</v>
+        <v>51262</v>
       </c>
       <c r="E78">
-        <v>203922</v>
+        <v>9538</v>
       </c>
       <c r="F78">
-        <v>70255</v>
+        <v>3495</v>
       </c>
       <c r="G78">
-        <v>26.9</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B79">
-        <v>25206</v>
+        <v>22473</v>
       </c>
       <c r="C79">
-        <v>55098</v>
+        <v>51506</v>
       </c>
       <c r="D79">
-        <v>67227</v>
+        <v>58239</v>
       </c>
       <c r="E79">
-        <v>139900</v>
+        <v>60485</v>
       </c>
       <c r="F79">
-        <v>53051</v>
+        <v>21343</v>
       </c>
       <c r="G79">
-        <v>34.4</v>
+        <v>27</v>
       </c>
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B80">
-        <v>16561</v>
+        <v>20263</v>
       </c>
       <c r="C80">
-        <v>38376</v>
+        <v>42081</v>
       </c>
       <c r="D80">
-        <v>51262</v>
+        <v>52177</v>
       </c>
       <c r="E80">
-        <v>9538</v>
+        <v>13900</v>
       </c>
       <c r="F80">
-        <v>3495</v>
+        <v>5044</v>
       </c>
       <c r="G80">
-        <v>20.9</v>
+        <v>16.3</v>
       </c>
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="B81">
-        <v>22473</v>
+        <v>15730</v>
       </c>
       <c r="C81">
-        <v>51506</v>
+        <v>32928</v>
       </c>
       <c r="D81">
-        <v>58239</v>
+        <v>40313</v>
       </c>
       <c r="E81">
-        <v>60485</v>
+        <v>15068</v>
       </c>
       <c r="F81">
-        <v>21343</v>
+        <v>5689</v>
       </c>
       <c r="G81">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B82">
-        <v>20263</v>
+        <v>15165</v>
       </c>
       <c r="C82">
-        <v>42081</v>
+        <v>29268</v>
       </c>
       <c r="D82">
-        <v>52177</v>
+        <v>36980</v>
       </c>
       <c r="E82">
-        <v>13900</v>
+        <v>16930</v>
       </c>
       <c r="F82">
-        <v>5044</v>
+        <v>6241</v>
       </c>
       <c r="G82">
-        <v>16.3</v>
+        <v>16.7</v>
       </c>
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="B83">
-        <v>15730</v>
+        <v>17629</v>
       </c>
       <c r="C83">
-        <v>32928</v>
+        <v>27686</v>
       </c>
       <c r="D83">
-        <v>40313</v>
+        <v>35876</v>
       </c>
       <c r="E83">
-        <v>15068</v>
+        <v>8340</v>
       </c>
       <c r="F83">
-        <v>5689</v>
+        <v>3192</v>
       </c>
       <c r="G83">
         <v>18</v>
@@ -2760,689 +2810,689 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="B84">
-        <v>15165</v>
+        <v>15659</v>
       </c>
       <c r="C84">
-        <v>29268</v>
+        <v>27607</v>
       </c>
       <c r="D84">
-        <v>36980</v>
+        <v>35750</v>
       </c>
       <c r="E84">
-        <v>16930</v>
+        <v>9980</v>
       </c>
       <c r="F84">
-        <v>6241</v>
+        <v>3347</v>
       </c>
       <c r="G84">
-        <v>16.7</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B85">
-        <v>17629</v>
+        <v>21598</v>
       </c>
       <c r="C85">
-        <v>27686</v>
+        <v>50717</v>
       </c>
       <c r="D85">
-        <v>35876</v>
+        <v>56038</v>
       </c>
       <c r="E85">
-        <v>8340</v>
+        <v>28669</v>
       </c>
       <c r="F85">
-        <v>3192</v>
+        <v>10586</v>
       </c>
       <c r="G85">
-        <v>18</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="B86">
-        <v>15659</v>
+        <v>17725</v>
       </c>
       <c r="C86">
-        <v>27607</v>
+        <v>37536</v>
       </c>
       <c r="D86">
-        <v>35750</v>
+        <v>42218</v>
       </c>
       <c r="E86">
-        <v>9980</v>
+        <v>18317</v>
       </c>
       <c r="F86">
-        <v>3347</v>
+        <v>6618</v>
       </c>
       <c r="G86">
-        <v>14.7</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="B87">
-        <v>21598</v>
+        <v>16894</v>
       </c>
       <c r="C87">
-        <v>50717</v>
+        <v>37522</v>
       </c>
       <c r="D87">
-        <v>56038</v>
+        <v>43162</v>
       </c>
       <c r="E87">
-        <v>28669</v>
+        <v>10078</v>
       </c>
       <c r="F87">
-        <v>10586</v>
+        <v>3608</v>
       </c>
       <c r="G87">
-        <v>27.6</v>
+        <v>25.4</v>
       </c>
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B88">
-        <v>17725</v>
+        <v>19387</v>
       </c>
       <c r="C88">
-        <v>37536</v>
+        <v>38280</v>
       </c>
       <c r="D88">
-        <v>42218</v>
+        <v>46466</v>
       </c>
       <c r="E88">
-        <v>18317</v>
+        <v>48434</v>
       </c>
       <c r="F88">
-        <v>6618</v>
+        <v>18641</v>
       </c>
       <c r="G88">
-        <v>23.6</v>
+        <v>23.1</v>
       </c>
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="B89">
-        <v>16894</v>
+        <v>23867</v>
       </c>
       <c r="C89">
-        <v>37522</v>
+        <v>59811</v>
       </c>
       <c r="D89">
-        <v>43162</v>
+        <v>67943</v>
       </c>
       <c r="E89">
-        <v>10078</v>
+        <v>28298</v>
       </c>
       <c r="F89">
-        <v>3608</v>
+        <v>9706</v>
       </c>
       <c r="G89">
-        <v>25.4</v>
+        <v>35.9</v>
       </c>
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="B90">
-        <v>19387</v>
+        <v>18662</v>
       </c>
       <c r="C90">
-        <v>38280</v>
+        <v>42674</v>
       </c>
       <c r="D90">
-        <v>46466</v>
+        <v>46818</v>
       </c>
       <c r="E90">
-        <v>48434</v>
+        <v>63453</v>
       </c>
       <c r="F90">
-        <v>18641</v>
+        <v>22155</v>
       </c>
       <c r="G90">
-        <v>23.1</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
       <c r="B91">
-        <v>23867</v>
+        <v>19627</v>
       </c>
       <c r="C91">
-        <v>59811</v>
+        <v>36399</v>
       </c>
       <c r="D91">
-        <v>67943</v>
+        <v>43872</v>
       </c>
       <c r="E91">
-        <v>28298</v>
+        <v>7996</v>
       </c>
       <c r="F91">
-        <v>9706</v>
+        <v>3281</v>
       </c>
       <c r="G91">
-        <v>35.9</v>
+        <v>21</v>
       </c>
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B92">
-        <v>18662</v>
+        <v>15068</v>
       </c>
       <c r="C92">
-        <v>42674</v>
+        <v>41186</v>
       </c>
       <c r="D92">
-        <v>46818</v>
+        <v>46654</v>
       </c>
       <c r="E92">
-        <v>63453</v>
+        <v>14464</v>
       </c>
       <c r="F92">
-        <v>22155</v>
+        <v>5023</v>
       </c>
       <c r="G92">
-        <v>27.6</v>
+        <v>25.2</v>
       </c>
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
       <c r="B93">
-        <v>19627</v>
+        <v>20041</v>
       </c>
       <c r="C93">
-        <v>36399</v>
+        <v>39096</v>
       </c>
       <c r="D93">
-        <v>43872</v>
+        <v>48296</v>
       </c>
       <c r="E93">
-        <v>7996</v>
+        <v>109233</v>
       </c>
       <c r="F93">
-        <v>3281</v>
+        <v>39747</v>
       </c>
       <c r="G93">
-        <v>21</v>
+        <v>32.299999999999997</v>
       </c>
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B94">
-        <v>15068</v>
+        <v>20088</v>
       </c>
       <c r="C94">
-        <v>41186</v>
+        <v>43394</v>
       </c>
       <c r="D94">
-        <v>46654</v>
+        <v>50318</v>
       </c>
       <c r="E94">
-        <v>14464</v>
+        <v>29966</v>
       </c>
       <c r="F94">
-        <v>5023</v>
+        <v>10989</v>
       </c>
       <c r="G94">
-        <v>25.2</v>
+        <v>34.700000000000003</v>
       </c>
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="B95">
-        <v>20041</v>
+        <v>12902</v>
       </c>
       <c r="C95">
-        <v>39096</v>
+        <v>27950</v>
       </c>
       <c r="D95">
-        <v>48296</v>
+        <v>37218</v>
       </c>
       <c r="E95">
-        <v>109233</v>
+        <v>14740</v>
       </c>
       <c r="F95">
-        <v>39747</v>
+        <v>4999</v>
       </c>
       <c r="G95">
-        <v>32.299999999999997</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="B96">
-        <v>20088</v>
+        <v>18975</v>
       </c>
       <c r="C96">
-        <v>43394</v>
+        <v>41343</v>
       </c>
       <c r="D96">
-        <v>50318</v>
+        <v>49713</v>
       </c>
       <c r="E96">
-        <v>29966</v>
+        <v>28120</v>
       </c>
       <c r="F96">
-        <v>10989</v>
+        <v>10508</v>
       </c>
       <c r="G96">
-        <v>34.700000000000003</v>
+        <v>23.3</v>
       </c>
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="B97">
-        <v>12902</v>
+        <v>17729</v>
       </c>
       <c r="C97">
-        <v>27950</v>
+        <v>31581</v>
       </c>
       <c r="D97">
-        <v>37218</v>
+        <v>51000</v>
       </c>
       <c r="E97">
-        <v>14740</v>
+        <v>8742</v>
       </c>
       <c r="F97">
-        <v>4999</v>
+        <v>3420</v>
       </c>
       <c r="G97">
-        <v>14.3</v>
+        <v>14.5</v>
       </c>
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B98">
-        <v>18975</v>
+        <v>17261</v>
       </c>
       <c r="C98">
-        <v>41343</v>
+        <v>35414</v>
       </c>
       <c r="D98">
-        <v>49713</v>
+        <v>42472</v>
       </c>
       <c r="E98">
-        <v>28120</v>
+        <v>21875</v>
       </c>
       <c r="F98">
-        <v>10508</v>
+        <v>8289</v>
       </c>
       <c r="G98">
-        <v>23.3</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="B99">
-        <v>17729</v>
+        <v>20964</v>
       </c>
       <c r="C99">
-        <v>31581</v>
+        <v>39075</v>
       </c>
       <c r="D99">
-        <v>51000</v>
+        <v>51765</v>
       </c>
       <c r="E99">
-        <v>8742</v>
+        <v>14333</v>
       </c>
       <c r="F99">
-        <v>3420</v>
+        <v>5971</v>
       </c>
       <c r="G99">
-        <v>14.5</v>
+        <v>23.2</v>
       </c>
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B100">
-        <v>17261</v>
+        <v>18295</v>
       </c>
       <c r="C100">
-        <v>35414</v>
+        <v>37845</v>
       </c>
       <c r="D100">
-        <v>42472</v>
+        <v>47126</v>
       </c>
       <c r="E100">
-        <v>21875</v>
+        <v>21992</v>
       </c>
       <c r="F100">
-        <v>8289</v>
+        <v>8522</v>
       </c>
       <c r="G100">
-        <v>21.3</v>
+        <v>15.6</v>
       </c>
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B101">
-        <v>20964</v>
+        <v>19895</v>
       </c>
       <c r="C101">
-        <v>39075</v>
+        <v>33196</v>
       </c>
       <c r="D101">
-        <v>51765</v>
+        <v>40685</v>
       </c>
       <c r="E101">
-        <v>14333</v>
+        <v>6125</v>
       </c>
       <c r="F101">
-        <v>5971</v>
+        <v>2426</v>
       </c>
       <c r="G101">
-        <v>23.2</v>
+        <v>18</v>
       </c>
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B102">
-        <v>18295</v>
+        <v>16322</v>
       </c>
       <c r="C102">
-        <v>37845</v>
+        <v>36198</v>
       </c>
       <c r="D102">
-        <v>47126</v>
+        <v>43930</v>
       </c>
       <c r="E102">
-        <v>21992</v>
+        <v>23498</v>
       </c>
       <c r="F102">
-        <v>8522</v>
+        <v>8055</v>
       </c>
       <c r="G102">
-        <v>15.6</v>
+        <v>17.600000000000001</v>
       </c>
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="B103">
-        <v>19895</v>
+        <v>23656</v>
       </c>
       <c r="C103">
-        <v>33196</v>
+        <v>48297</v>
       </c>
       <c r="D103">
-        <v>40685</v>
+        <v>61110</v>
       </c>
       <c r="E103">
-        <v>6125</v>
+        <v>26424</v>
       </c>
       <c r="F103">
-        <v>2426</v>
+        <v>9662</v>
       </c>
       <c r="G103">
-        <v>18</v>
+        <v>28.2</v>
       </c>
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B104">
-        <v>16322</v>
+        <v>17168</v>
       </c>
       <c r="C104">
-        <v>36198</v>
+        <v>35182</v>
       </c>
       <c r="D104">
-        <v>43930</v>
+        <v>45989</v>
       </c>
       <c r="E104">
-        <v>23498</v>
+        <v>9123</v>
       </c>
       <c r="F104">
-        <v>8055</v>
+        <v>3287</v>
       </c>
       <c r="G104">
-        <v>17.600000000000001</v>
+        <v>21</v>
       </c>
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B105">
-        <v>23656</v>
+        <v>27732</v>
       </c>
       <c r="C105">
-        <v>48297</v>
+        <v>45817</v>
       </c>
       <c r="D105">
-        <v>61110</v>
+        <v>57724</v>
       </c>
       <c r="E105">
-        <v>26424</v>
+        <v>17868</v>
       </c>
       <c r="F105">
-        <v>9662</v>
+        <v>6660</v>
       </c>
       <c r="G105">
-        <v>28.2</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B106">
-        <v>17168</v>
+        <v>16925</v>
       </c>
       <c r="C106">
-        <v>35182</v>
+        <v>38226</v>
       </c>
       <c r="D106">
-        <v>45989</v>
+        <v>45420</v>
       </c>
       <c r="E106">
-        <v>9123</v>
+        <v>39628</v>
       </c>
       <c r="F106">
-        <v>3287</v>
+        <v>14080</v>
       </c>
       <c r="G106">
-        <v>21</v>
+        <v>16</v>
       </c>
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="B107">
-        <v>27732</v>
+        <v>22514</v>
       </c>
       <c r="C107">
-        <v>45817</v>
+        <v>41331</v>
       </c>
       <c r="D107">
-        <v>57724</v>
+        <v>50771</v>
       </c>
       <c r="E107">
-        <v>17868</v>
+        <v>189885</v>
       </c>
       <c r="F107">
-        <v>6660</v>
+        <v>74081</v>
       </c>
       <c r="G107">
-        <v>27.7</v>
+        <v>33.9</v>
       </c>
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="B108">
-        <v>16925</v>
+        <v>21583</v>
       </c>
       <c r="C108">
-        <v>38226</v>
+        <v>52361</v>
       </c>
       <c r="D108">
-        <v>45420</v>
+        <v>56519</v>
       </c>
       <c r="E108">
-        <v>39628</v>
+        <v>99958</v>
       </c>
       <c r="F108">
-        <v>14080</v>
+        <v>34390</v>
       </c>
       <c r="G108">
-        <v>16</v>
+        <v>27.6</v>
       </c>
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B109">
-        <v>22514</v>
+        <v>34271</v>
       </c>
       <c r="C109">
-        <v>41331</v>
+        <v>74352</v>
       </c>
       <c r="D109">
-        <v>50771</v>
+        <v>85371</v>
       </c>
       <c r="E109">
-        <v>189885</v>
+        <v>32808</v>
       </c>
       <c r="F109">
-        <v>74081</v>
+        <v>11622</v>
       </c>
       <c r="G109">
-        <v>33.9</v>
+        <v>53.8</v>
       </c>
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="B110">
-        <v>21583</v>
+        <v>17572</v>
       </c>
       <c r="C110">
-        <v>52361</v>
+        <v>39319</v>
       </c>
       <c r="D110">
-        <v>56519</v>
+        <v>52955</v>
       </c>
       <c r="E110">
-        <v>99958</v>
+        <v>14899</v>
       </c>
       <c r="F110">
-        <v>34390</v>
+        <v>5647</v>
       </c>
       <c r="G110">
-        <v>27.6</v>
+        <v>23.6</v>
       </c>
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="B111">
-        <v>34271</v>
+        <v>23450</v>
       </c>
       <c r="C111">
-        <v>74352</v>
+        <v>62348</v>
       </c>
       <c r="D111">
-        <v>85371</v>
+        <v>67117</v>
       </c>
       <c r="E111">
-        <v>32808</v>
+        <v>142324</v>
       </c>
       <c r="F111">
-        <v>11622</v>
+        <v>48105</v>
       </c>
       <c r="G111">
-        <v>53.8</v>
+        <v>32.5</v>
       </c>
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B112">
-        <v>17572</v>
+        <v>18681</v>
       </c>
       <c r="C112">
-        <v>39319</v>
+        <v>41014</v>
       </c>
       <c r="D112">
-        <v>52955</v>
+        <v>53708</v>
       </c>
       <c r="E112">
-        <v>14899</v>
+        <v>27695</v>
       </c>
       <c r="F112">
-        <v>5647</v>
+        <v>9958</v>
       </c>
       <c r="G112">
-        <v>23.6</v>
+        <v>27.2</v>
       </c>
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B113">
-        <v>23450</v>
+        <v>25892</v>
       </c>
       <c r="C113">
-        <v>62348</v>
+        <v>49945</v>
       </c>
       <c r="D113">
-        <v>67117</v>
+        <v>59955</v>
       </c>
       <c r="E113">
-        <v>142324</v>
+        <v>29431</v>
       </c>
       <c r="F113">
-        <v>48105</v>
+        <v>11291</v>
       </c>
       <c r="G113">
         <v>32.5</v>
@@ -3450,1128 +3500,1082 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="B114">
-        <v>18681</v>
+        <v>18283</v>
       </c>
       <c r="C114">
-        <v>41014</v>
+        <v>37062</v>
       </c>
       <c r="D114">
-        <v>53708</v>
+        <v>47157</v>
       </c>
       <c r="E114">
-        <v>27695</v>
+        <v>18758</v>
       </c>
       <c r="F114">
-        <v>9958</v>
+        <v>7083</v>
       </c>
       <c r="G114">
-        <v>27.2</v>
+        <v>20.6</v>
       </c>
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B115">
-        <v>25892</v>
+        <v>21051</v>
       </c>
       <c r="C115">
-        <v>49945</v>
+        <v>53213</v>
       </c>
       <c r="D115">
-        <v>59955</v>
+        <v>57458</v>
       </c>
       <c r="E115">
-        <v>29431</v>
+        <v>17869</v>
       </c>
       <c r="F115">
-        <v>11291</v>
+        <v>6187</v>
       </c>
       <c r="G115">
-        <v>32.5</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="B116">
-        <v>18283</v>
+        <v>18214</v>
       </c>
       <c r="C116">
-        <v>37062</v>
+        <v>38646</v>
       </c>
       <c r="D116">
-        <v>47157</v>
+        <v>43172</v>
       </c>
       <c r="E116">
-        <v>18758</v>
+        <v>41475</v>
       </c>
       <c r="F116">
-        <v>7083</v>
+        <v>15092</v>
       </c>
       <c r="G116">
-        <v>20.6</v>
+        <v>18.7</v>
       </c>
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B117">
-        <v>21051</v>
+        <v>16621</v>
       </c>
       <c r="C117">
-        <v>53213</v>
+        <v>36262</v>
       </c>
       <c r="D117">
-        <v>57458</v>
+        <v>46850</v>
       </c>
       <c r="E117">
-        <v>17869</v>
+        <v>12010</v>
       </c>
       <c r="F117">
-        <v>6187</v>
+        <v>4475</v>
       </c>
       <c r="G117">
-        <v>22.1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B118">
-        <v>18214</v>
+        <v>25576</v>
       </c>
       <c r="C118">
-        <v>38646</v>
+        <v>41529</v>
       </c>
       <c r="D118">
-        <v>43172</v>
+        <v>49814</v>
       </c>
       <c r="E118">
-        <v>41475</v>
+        <v>21218</v>
       </c>
       <c r="F118">
-        <v>15092</v>
+        <v>8601</v>
       </c>
       <c r="G118">
-        <v>18.7</v>
+        <v>26</v>
       </c>
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B119">
-        <v>16621</v>
+        <v>13642</v>
       </c>
       <c r="C119">
-        <v>36262</v>
+        <v>28912</v>
       </c>
       <c r="D119">
-        <v>46850</v>
+        <v>34342</v>
       </c>
       <c r="E119">
-        <v>12010</v>
+        <v>2513</v>
       </c>
       <c r="F119">
-        <v>4475</v>
+        <v>1053</v>
       </c>
       <c r="G119">
-        <v>20</v>
+        <v>10.8</v>
       </c>
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="B120">
-        <v>25576</v>
+        <v>22471</v>
       </c>
       <c r="C120">
-        <v>41529</v>
+        <v>34406</v>
       </c>
       <c r="D120">
-        <v>49814</v>
+        <v>50410</v>
       </c>
       <c r="E120">
-        <v>21218</v>
+        <v>16276</v>
       </c>
       <c r="F120">
-        <v>8601</v>
+        <v>6780</v>
       </c>
       <c r="G120">
-        <v>26</v>
+        <v>32.299999999999997</v>
       </c>
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B121">
-        <v>13642</v>
+        <v>17632</v>
       </c>
       <c r="C121">
-        <v>28912</v>
+        <v>26194</v>
       </c>
       <c r="D121">
-        <v>34342</v>
+        <v>29800</v>
       </c>
       <c r="E121">
-        <v>2513</v>
+        <v>7719</v>
       </c>
       <c r="F121">
-        <v>1053</v>
+        <v>3187</v>
       </c>
       <c r="G121">
-        <v>10.8</v>
+        <v>18.3</v>
       </c>
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B122">
-        <v>22471</v>
+        <v>20604</v>
       </c>
       <c r="C122">
-        <v>34406</v>
+        <v>37882</v>
       </c>
       <c r="D122">
-        <v>50410</v>
+        <v>45220</v>
       </c>
       <c r="E122">
-        <v>16276</v>
+        <v>200549</v>
       </c>
       <c r="F122">
-        <v>6780</v>
+        <v>76924</v>
       </c>
       <c r="G122">
-        <v>32.299999999999997</v>
+        <v>28.9</v>
       </c>
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="B123">
-        <v>17632</v>
+        <v>24367</v>
       </c>
       <c r="C123">
-        <v>26194</v>
+        <v>55779</v>
       </c>
       <c r="D123">
-        <v>29800</v>
+        <v>63167</v>
       </c>
       <c r="E123">
-        <v>7719</v>
+        <v>85215</v>
       </c>
       <c r="F123">
-        <v>3187</v>
+        <v>30027</v>
       </c>
       <c r="G123">
-        <v>18.3</v>
+        <v>34.700000000000003</v>
       </c>
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B124">
-        <v>20604</v>
+        <v>16122</v>
       </c>
       <c r="C124">
-        <v>37882</v>
+        <v>35096</v>
       </c>
       <c r="D124">
-        <v>45220</v>
+        <v>47234</v>
       </c>
       <c r="E124">
-        <v>200549</v>
+        <v>5010</v>
       </c>
       <c r="F124">
-        <v>76924</v>
+        <v>1872</v>
       </c>
       <c r="G124">
-        <v>28.9</v>
+        <v>22.5</v>
       </c>
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="B125">
-        <v>24367</v>
+        <v>16189</v>
       </c>
       <c r="C125">
-        <v>55779</v>
+        <v>32155</v>
       </c>
       <c r="D125">
-        <v>63167</v>
+        <v>44244</v>
       </c>
       <c r="E125">
-        <v>85215</v>
+        <v>14593</v>
       </c>
       <c r="F125">
-        <v>30027</v>
+        <v>5596</v>
       </c>
       <c r="G125">
-        <v>34.700000000000003</v>
+        <v>20.7</v>
       </c>
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="B126">
-        <v>16122</v>
+        <v>19263</v>
       </c>
       <c r="C126">
-        <v>35096</v>
+        <v>32666</v>
       </c>
       <c r="D126">
-        <v>47234</v>
+        <v>38339</v>
       </c>
       <c r="E126">
-        <v>5010</v>
+        <v>8729</v>
       </c>
       <c r="F126">
-        <v>1872</v>
+        <v>3509</v>
       </c>
       <c r="G126">
-        <v>22.5</v>
+        <v>20.8</v>
       </c>
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B127">
-        <v>16189</v>
+        <v>19607</v>
       </c>
       <c r="C127">
-        <v>32155</v>
+        <v>41100</v>
       </c>
       <c r="D127">
-        <v>44244</v>
+        <v>49640</v>
       </c>
       <c r="E127">
-        <v>14593</v>
+        <v>64073</v>
       </c>
       <c r="F127">
-        <v>5596</v>
+        <v>23565</v>
       </c>
       <c r="G127">
-        <v>20.7</v>
+        <v>21.8</v>
       </c>
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="B128">
-        <v>19263</v>
+        <v>18285</v>
       </c>
       <c r="C128">
-        <v>32666</v>
+        <v>34938</v>
       </c>
       <c r="D128">
-        <v>38339</v>
+        <v>41768</v>
       </c>
       <c r="E128">
-        <v>8729</v>
+        <v>26175</v>
       </c>
       <c r="F128">
-        <v>3509</v>
+        <v>10289</v>
       </c>
       <c r="G128">
-        <v>20.8</v>
+        <v>24.5</v>
       </c>
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="B129">
-        <v>19607</v>
+        <v>15612</v>
       </c>
       <c r="C129">
-        <v>41100</v>
+        <v>30954</v>
       </c>
       <c r="D129">
-        <v>49640</v>
+        <v>41673</v>
       </c>
       <c r="E129">
-        <v>64073</v>
+        <v>6058</v>
       </c>
       <c r="F129">
-        <v>23565</v>
+        <v>1862</v>
       </c>
       <c r="G129">
-        <v>21.8</v>
+        <v>14.7</v>
       </c>
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B130">
-        <v>18285</v>
+        <v>17436</v>
       </c>
       <c r="C130">
-        <v>34938</v>
+        <v>32430</v>
       </c>
       <c r="D130">
-        <v>41768</v>
+        <v>41371</v>
       </c>
       <c r="E130">
-        <v>26175</v>
+        <v>32819</v>
       </c>
       <c r="F130">
-        <v>10289</v>
+        <v>12123</v>
       </c>
       <c r="G130">
-        <v>24.5</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="B131">
-        <v>15612</v>
+        <v>18007</v>
       </c>
       <c r="C131">
-        <v>30954</v>
+        <v>33873</v>
       </c>
       <c r="D131">
-        <v>41673</v>
+        <v>43694</v>
       </c>
       <c r="E131">
-        <v>6058</v>
+        <v>6865</v>
       </c>
       <c r="F131">
-        <v>1862</v>
+        <v>2832</v>
       </c>
       <c r="G131">
-        <v>14.7</v>
+        <v>18.899999999999999</v>
       </c>
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="B132">
-        <v>17436</v>
+        <v>13955</v>
       </c>
       <c r="C132">
-        <v>32430</v>
+        <v>22188</v>
       </c>
       <c r="D132">
-        <v>41371</v>
+        <v>29375</v>
       </c>
       <c r="E132">
-        <v>32819</v>
+        <v>1717</v>
       </c>
       <c r="F132">
-        <v>12123</v>
+        <v>759</v>
       </c>
       <c r="G132">
-        <v>26.7</v>
+        <v>12.9</v>
       </c>
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B133">
-        <v>18007</v>
+        <v>16742</v>
       </c>
       <c r="C133">
-        <v>33873</v>
+        <v>38522</v>
       </c>
       <c r="D133">
-        <v>43694</v>
+        <v>45601</v>
       </c>
       <c r="E133">
-        <v>6865</v>
+        <v>25520</v>
       </c>
       <c r="F133">
-        <v>2832</v>
+        <v>8210</v>
       </c>
       <c r="G133">
-        <v>18.899999999999999</v>
+        <v>17.899999999999999</v>
       </c>
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="B134">
-        <v>13955</v>
+        <v>14693</v>
       </c>
       <c r="C134">
-        <v>22188</v>
+        <v>25237</v>
       </c>
       <c r="D134">
-        <v>29375</v>
+        <v>35819</v>
       </c>
       <c r="E134">
-        <v>1717</v>
+        <v>8906</v>
       </c>
       <c r="F134">
-        <v>759</v>
+        <v>3522</v>
       </c>
       <c r="G134">
-        <v>12.9</v>
+        <v>17.3</v>
       </c>
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="B135">
-        <v>16742</v>
+        <v>13420</v>
       </c>
       <c r="C135">
-        <v>38522</v>
+        <v>23876</v>
       </c>
       <c r="D135">
-        <v>45601</v>
+        <v>36109</v>
       </c>
       <c r="E135">
-        <v>25520</v>
+        <v>16500</v>
       </c>
       <c r="F135">
-        <v>8210</v>
+        <v>5543</v>
       </c>
       <c r="G135">
-        <v>17.899999999999999</v>
+        <v>14.3</v>
       </c>
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
       <c r="B136">
-        <v>14693</v>
+        <v>15553</v>
       </c>
       <c r="C136">
-        <v>25237</v>
+        <v>27909</v>
       </c>
       <c r="D136">
-        <v>35819</v>
+        <v>35663</v>
       </c>
       <c r="E136">
-        <v>8906</v>
+        <v>9315</v>
       </c>
       <c r="F136">
-        <v>3522</v>
+        <v>3519</v>
       </c>
       <c r="G136">
-        <v>17.3</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B137">
-        <v>13420</v>
+        <v>21261</v>
       </c>
       <c r="C137">
-        <v>23876</v>
+        <v>35797</v>
       </c>
       <c r="D137">
-        <v>36109</v>
+        <v>46333</v>
       </c>
       <c r="E137">
-        <v>16500</v>
+        <v>44720</v>
       </c>
       <c r="F137">
-        <v>5543</v>
+        <v>17573</v>
       </c>
       <c r="G137">
-        <v>14.3</v>
+        <v>27.7</v>
       </c>
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="B138">
-        <v>15553</v>
+        <v>18394</v>
       </c>
       <c r="C138">
-        <v>27909</v>
+        <v>36847</v>
       </c>
       <c r="D138">
-        <v>35663</v>
+        <v>45376</v>
       </c>
       <c r="E138">
-        <v>9315</v>
+        <v>40118</v>
       </c>
       <c r="F138">
-        <v>3519</v>
+        <v>14836</v>
       </c>
       <c r="G138">
-        <v>20.9</v>
+        <v>28.7</v>
       </c>
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="B139">
-        <v>21261</v>
+        <v>17974</v>
       </c>
       <c r="C139">
-        <v>35797</v>
+        <v>31635</v>
       </c>
       <c r="D139">
-        <v>46333</v>
+        <v>44266</v>
       </c>
       <c r="E139">
-        <v>44720</v>
+        <v>27223</v>
       </c>
       <c r="F139">
-        <v>17573</v>
+        <v>10375</v>
       </c>
       <c r="G139">
-        <v>27.7</v>
+        <v>22.1</v>
       </c>
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B140">
-        <v>18394</v>
+        <v>21527</v>
       </c>
       <c r="C140">
-        <v>36847</v>
+        <v>39540</v>
       </c>
       <c r="D140">
-        <v>45376</v>
+        <v>48020</v>
       </c>
       <c r="E140">
-        <v>40118</v>
+        <v>10471</v>
       </c>
       <c r="F140">
-        <v>14836</v>
+        <v>4510</v>
       </c>
       <c r="G140">
-        <v>28.7</v>
+        <v>34</v>
       </c>
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="B141">
-        <v>17974</v>
+        <v>16710</v>
       </c>
       <c r="C141">
-        <v>31635</v>
+        <v>36467</v>
       </c>
       <c r="D141">
-        <v>44266</v>
+        <v>48110</v>
       </c>
       <c r="E141">
-        <v>27223</v>
+        <v>6885</v>
       </c>
       <c r="F141">
-        <v>10375</v>
+        <v>2543</v>
       </c>
       <c r="G141">
-        <v>22.1</v>
+        <v>21.3</v>
       </c>
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="B142">
-        <v>21527</v>
+        <v>19699</v>
       </c>
       <c r="C142">
-        <v>39540</v>
+        <v>41770</v>
       </c>
       <c r="D142">
-        <v>48020</v>
+        <v>50625</v>
       </c>
       <c r="E142">
-        <v>10471</v>
+        <v>67044</v>
       </c>
       <c r="F142">
-        <v>4510</v>
+        <v>24828</v>
       </c>
       <c r="G142">
-        <v>34</v>
+        <v>25.3</v>
       </c>
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B143">
-        <v>16710</v>
+        <v>15973</v>
       </c>
       <c r="C143">
-        <v>36467</v>
+        <v>30763</v>
       </c>
       <c r="D143">
-        <v>48110</v>
+        <v>40446</v>
       </c>
       <c r="E143">
-        <v>6885</v>
+        <v>8930</v>
       </c>
       <c r="F143">
-        <v>2543</v>
+        <v>3339</v>
       </c>
       <c r="G143">
-        <v>21.3</v>
+        <v>20.100000000000001</v>
       </c>
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B144">
-        <v>19699</v>
+        <v>15904</v>
       </c>
       <c r="C144">
-        <v>41770</v>
+        <v>26521</v>
       </c>
       <c r="D144">
-        <v>50625</v>
+        <v>31324</v>
       </c>
       <c r="E144">
-        <v>67044</v>
+        <v>9023</v>
       </c>
       <c r="F144">
-        <v>24828</v>
+        <v>3634</v>
       </c>
       <c r="G144">
-        <v>25.3</v>
+        <v>16.2</v>
       </c>
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B145">
-        <v>15973</v>
+        <v>24182</v>
       </c>
       <c r="C145">
-        <v>30763</v>
+        <v>41298</v>
       </c>
       <c r="D145">
-        <v>40446</v>
+        <v>50772</v>
       </c>
       <c r="E145">
-        <v>8930</v>
+        <v>21356</v>
       </c>
       <c r="F145">
-        <v>3339</v>
+        <v>9116</v>
       </c>
       <c r="G145">
-        <v>20.100000000000001</v>
+        <v>31.9</v>
       </c>
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B146">
-        <v>15904</v>
+        <v>17398</v>
       </c>
       <c r="C146">
-        <v>26521</v>
+        <v>34509</v>
       </c>
       <c r="D146">
-        <v>31324</v>
+        <v>42737</v>
       </c>
       <c r="E146">
-        <v>9023</v>
+        <v>27153</v>
       </c>
       <c r="F146">
-        <v>3634</v>
+        <v>10716</v>
       </c>
       <c r="G146">
-        <v>16.2</v>
+        <v>20.9</v>
       </c>
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>145</v>
+        <v>147</v>
       </c>
       <c r="B147">
-        <v>24182</v>
+        <v>19440</v>
       </c>
       <c r="C147">
-        <v>41298</v>
+        <v>38723</v>
       </c>
       <c r="D147">
-        <v>50772</v>
+        <v>46307</v>
       </c>
       <c r="E147">
-        <v>21356</v>
+        <v>68756</v>
       </c>
       <c r="F147">
-        <v>9116</v>
+        <v>26497</v>
       </c>
       <c r="G147">
-        <v>31.9</v>
+        <v>22.2</v>
       </c>
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B148">
-        <v>17398</v>
+        <v>22521</v>
       </c>
       <c r="C148">
-        <v>34509</v>
+        <v>51721</v>
       </c>
       <c r="D148">
-        <v>42737</v>
+        <v>58750</v>
       </c>
       <c r="E148">
-        <v>27153</v>
+        <v>83768</v>
       </c>
       <c r="F148">
-        <v>10716</v>
+        <v>29583</v>
       </c>
       <c r="G148">
-        <v>20.9</v>
+        <v>26.7</v>
       </c>
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="B149">
-        <v>19440</v>
+        <v>18295</v>
       </c>
       <c r="C149">
-        <v>38723</v>
+        <v>35517</v>
       </c>
       <c r="D149">
-        <v>46307</v>
+        <v>47609</v>
       </c>
       <c r="E149">
-        <v>68756</v>
+        <v>36312</v>
       </c>
       <c r="F149">
-        <v>26497</v>
+        <v>13654</v>
       </c>
       <c r="G149">
-        <v>22.2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B150">
-        <v>22521</v>
+        <v>15987</v>
       </c>
       <c r="C150">
-        <v>51721</v>
+        <v>31043</v>
       </c>
       <c r="D150">
-        <v>58750</v>
+        <v>36925</v>
       </c>
       <c r="E150">
-        <v>83768</v>
+        <v>5834</v>
       </c>
       <c r="F150">
-        <v>29583</v>
+        <v>2315</v>
       </c>
       <c r="G150">
-        <v>26.7</v>
+        <v>17.100000000000001</v>
       </c>
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="B151">
-        <v>18295</v>
+        <v>15033</v>
       </c>
       <c r="C151">
-        <v>35517</v>
+        <v>31382</v>
       </c>
       <c r="D151">
-        <v>47609</v>
+        <v>41055</v>
       </c>
       <c r="E151">
-        <v>36312</v>
+        <v>21187</v>
       </c>
       <c r="F151">
-        <v>13654</v>
+        <v>7547</v>
       </c>
       <c r="G151">
-        <v>20</v>
+        <v>19.5</v>
       </c>
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="B152">
-        <v>15987</v>
+        <v>18393</v>
       </c>
       <c r="C152">
-        <v>31043</v>
+        <v>37340</v>
       </c>
       <c r="D152">
-        <v>36925</v>
+        <v>45649</v>
       </c>
       <c r="E152">
-        <v>5834</v>
+        <v>30099</v>
       </c>
       <c r="F152">
-        <v>2315</v>
+        <v>10562</v>
       </c>
       <c r="G152">
-        <v>17.100000000000001</v>
+        <v>21.9</v>
       </c>
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B153">
-        <v>15033</v>
+        <v>16295</v>
       </c>
       <c r="C153">
-        <v>31382</v>
+        <v>25708</v>
       </c>
       <c r="D153">
-        <v>41055</v>
+        <v>40441</v>
       </c>
       <c r="E153">
-        <v>21187</v>
+        <v>2799</v>
       </c>
       <c r="F153">
-        <v>7547</v>
+        <v>1119</v>
       </c>
       <c r="G153">
-        <v>19.5</v>
+        <v>17.399999999999999</v>
       </c>
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="B154">
-        <v>18393</v>
+        <v>10043</v>
       </c>
       <c r="C154">
-        <v>37340</v>
+        <v>35422</v>
       </c>
       <c r="D154">
-        <v>45649</v>
+        <v>45042</v>
       </c>
       <c r="E154">
-        <v>30099</v>
+        <v>7421</v>
       </c>
       <c r="F154">
-        <v>10562</v>
+        <v>2152</v>
       </c>
       <c r="G154">
-        <v>21.9</v>
+        <v>12</v>
       </c>
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="B155">
-        <v>16295</v>
+        <v>23680</v>
       </c>
       <c r="C155">
-        <v>25708</v>
+        <v>41756</v>
       </c>
       <c r="D155">
-        <v>40441</v>
+        <v>50981</v>
       </c>
       <c r="E155">
-        <v>2799</v>
+        <v>27144</v>
       </c>
       <c r="F155">
-        <v>1119</v>
+        <v>10646</v>
       </c>
       <c r="G155">
-        <v>17.399999999999999</v>
+        <v>29.6</v>
       </c>
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B156">
-        <v>10043</v>
+        <v>19780</v>
       </c>
       <c r="C156">
-        <v>35422</v>
+        <v>42345</v>
       </c>
       <c r="D156">
-        <v>45042</v>
+        <v>48991</v>
       </c>
       <c r="E156">
-        <v>7421</v>
+        <v>102599</v>
       </c>
       <c r="F156">
-        <v>2152</v>
+        <v>35180</v>
       </c>
       <c r="G156">
-        <v>12</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="B157">
-        <v>23680</v>
+        <v>12692</v>
       </c>
       <c r="C157">
-        <v>41756</v>
+        <v>30784</v>
       </c>
       <c r="D157">
-        <v>50981</v>
+        <v>40552</v>
       </c>
       <c r="E157">
-        <v>27144</v>
+        <v>9255</v>
       </c>
       <c r="F157">
-        <v>10646</v>
+        <v>2891</v>
       </c>
       <c r="G157">
-        <v>29.6</v>
+        <v>14</v>
       </c>
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="B158">
-        <v>19780</v>
+        <v>16993</v>
       </c>
       <c r="C158">
-        <v>42345</v>
+        <v>28022</v>
       </c>
       <c r="D158">
-        <v>48991</v>
+        <v>39109</v>
       </c>
       <c r="E158">
-        <v>102599</v>
+        <v>10593</v>
       </c>
       <c r="F158">
-        <v>35180</v>
+        <v>4263</v>
       </c>
       <c r="G158">
-        <v>18.8</v>
+        <v>18.100000000000001</v>
       </c>
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B159">
-        <v>12692</v>
+        <v>17929</v>
       </c>
       <c r="C159">
-        <v>30784</v>
+        <v>37902</v>
       </c>
       <c r="D159">
-        <v>40552</v>
+        <v>49138</v>
       </c>
       <c r="E159">
-        <v>9255</v>
+        <v>9563</v>
       </c>
       <c r="F159">
-        <v>2891</v>
+        <v>3666</v>
       </c>
       <c r="G159">
-        <v>14</v>
+        <v>14.2</v>
       </c>
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="B160">
-        <v>16993</v>
+        <v>18348</v>
       </c>
       <c r="C160">
-        <v>28022</v>
+        <v>38670</v>
       </c>
       <c r="D160">
-        <v>39109</v>
+        <v>46791</v>
       </c>
       <c r="E160">
-        <v>10593</v>
+        <v>21679</v>
       </c>
       <c r="F160">
-        <v>4263</v>
+        <v>8214</v>
       </c>
       <c r="G160">
-        <v>18.100000000000001</v>
-      </c>
-    </row>
-    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A161" t="s">
-        <v>159</v>
-      </c>
-      <c r="B161">
-        <v>17929</v>
-      </c>
-      <c r="C161">
-        <v>37902</v>
-      </c>
-      <c r="D161">
-        <v>49138</v>
-      </c>
-      <c r="E161">
-        <v>9563</v>
-      </c>
-      <c r="F161">
-        <v>3666</v>
-      </c>
-      <c r="G161">
-        <v>14.2</v>
-      </c>
-    </row>
-    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A162" t="s">
-        <v>160</v>
-      </c>
-      <c r="B162">
-        <v>18348</v>
-      </c>
-      <c r="C162">
-        <v>38670</v>
-      </c>
-      <c r="D162">
-        <v>46791</v>
-      </c>
-      <c r="E162">
-        <v>21679</v>
-      </c>
-      <c r="F162">
-        <v>8214</v>
-      </c>
-      <c r="G162">
         <v>18</v>
       </c>
     </row>

</xml_diff>